<commit_message>
UI added (java FX)
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="62">
-  <si>
-    <t>Count of Invalid Options: 5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
+  <si>
+    <t>Count of Invalid Options: 4</t>
   </si>
   <si>
     <t>Error Log</t>
@@ -74,10 +74,10 @@
     <t>Meta product has errors</t>
   </si>
   <si>
-    <t>Option1 Value cannot be empty when Option1 Name is present</t>
-  </si>
-  <si>
-    <t>alphabet-keychain-with-leather-tasselgh</t>
+    <t>Invalid Option2 Name: Alphabet</t>
+  </si>
+  <si>
+    <t>alphabet-kh-leather-tassel</t>
   </si>
   <si>
     <t>ALPHABET KEYCHAIN WITH LEATHER TASSEL</t>
@@ -89,7 +89,10 @@
     <t>Colour</t>
   </si>
   <si>
-    <t>size</t>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Alphabet</t>
   </si>
   <si>
     <t>A</t>
@@ -98,18 +101,6 @@
     <t>AB234</t>
   </si>
   <si>
-    <t>Invalid Option2 Name: Alphabet</t>
-  </si>
-  <si>
-    <t>alphabet-kh-leather-tassel</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Alphabet</t>
-  </si>
-  <si>
     <t>Invalid Option1 Name: NG5625</t>
   </si>
   <si>
@@ -143,37 +134,19 @@
     <t>Count of Other Errors: 2</t>
   </si>
   <si>
-    <t>Valid title option must have only one record: 2 found.</t>
+    <t>Only one meta product with Option1 Name 'Title' and Option1 Value 'Default Title' is allowed per handle.</t>
   </si>
   <si>
     <t>alphabet-keychain-with-leather-tassel</t>
   </si>
   <si>
-    <t>ALPHABfvbdbdfbET KEYCHAIN WITH LEATHER TASSEL</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>ABCGF55</t>
-  </si>
-  <si>
-    <t>fggfnfhgn</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>AB2gbf34</t>
-  </si>
-  <si>
-    <t>Count of Invalid - Duplicate SKUs: 1</t>
-  </si>
-  <si>
-    <t>Duplicate SKU found</t>
-  </si>
-  <si>
-    <t>Count of Successful Records: 2</t>
+    <t>ABCDDFGH5</t>
+  </si>
+  <si>
+    <t>Count of Invalid - Duplicate SKUs: 0</t>
+  </si>
+  <si>
+    <t>Count of Successful Records: 0</t>
   </si>
   <si>
     <t>Option1 Name</t>
@@ -186,21 +159,6 @@
   </si>
   <si>
     <t>Option2 Value</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>ABdfg234</t>
-  </si>
-  <si>
-    <t>alphabet-keychain-with-leather-tasgfgfsel</t>
-  </si>
-  <si>
-    <t>gfbhnmymymym</t>
-  </si>
-  <si>
-    <t>fdvgbnh5253</t>
   </si>
 </sst>
 </file>
@@ -245,7 +203,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -337,16 +295,16 @@
         <v>23</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s" s="0">
         <v>18</v>
@@ -354,31 +312,31 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s" s="0">
         <v>18</v>
@@ -386,65 +344,33 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="E6" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="F6" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="G6" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="H6" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="I6" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="G6" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>39</v>
-      </c>
       <c r="J6" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="J7" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -463,7 +389,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
@@ -500,31 +426,31 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>15</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>15</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="J3" t="s" s="0">
         <v>15</v>
@@ -532,31 +458,31 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>15</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>15</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s" s="0">
         <v>15</v>
@@ -569,7 +495,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -577,7 +503,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
@@ -610,38 +536,6 @@
       </c>
       <c r="J2" t="s" s="0">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -651,7 +545,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -659,7 +553,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2">
@@ -673,80 +567,22 @@
         <v>4</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="I2" t="s" s="0">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>